<commit_message>
140511 2 new problems
</commit_message>
<xml_diff>
--- a/jzoffer.xlsx
+++ b/jzoffer.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\zjoffer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5115"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>面试题1</t>
   </si>
@@ -233,259 +228,268 @@
     <t>把数组排成最小的数</t>
   </si>
   <si>
+    <t>丑数</t>
+  </si>
+  <si>
+    <t>面试题35</t>
+  </si>
+  <si>
+    <t>第一个只出现一次的字符</t>
+  </si>
+  <si>
+    <t>面试题36</t>
+  </si>
+  <si>
+    <t>数组中的逆序对</t>
+  </si>
+  <si>
+    <t>面试题37</t>
+  </si>
+  <si>
+    <t>两个链表的第一个公共结点</t>
+  </si>
+  <si>
+    <t>面试题38</t>
+  </si>
+  <si>
+    <t>数字在排序数组中出现的次数</t>
+  </si>
+  <si>
+    <t>面试题39</t>
+  </si>
+  <si>
+    <t>二叉树的深度</t>
+  </si>
+  <si>
+    <t>面试题40</t>
+  </si>
+  <si>
+    <t>数组中只出现一次的数字</t>
+  </si>
+  <si>
+    <t>面试题41</t>
+  </si>
+  <si>
+    <t>和为S的两个数字</t>
+  </si>
+  <si>
+    <t>和为S的连续正数序列</t>
+  </si>
+  <si>
+    <t>面试题42</t>
+  </si>
+  <si>
+    <t>翻转单词顺序</t>
+  </si>
+  <si>
+    <t>左旋转字符串</t>
+  </si>
+  <si>
+    <t>面试题43</t>
+  </si>
+  <si>
+    <t>N个骰子的点数</t>
+  </si>
+  <si>
+    <t>面试题44</t>
+  </si>
+  <si>
+    <t>扑克牌的顺子</t>
+  </si>
+  <si>
+    <t>面试题45</t>
+  </si>
+  <si>
+    <t>圆圈中最后剩下的数</t>
+  </si>
+  <si>
+    <t>面试题46</t>
+  </si>
+  <si>
+    <t>求1+2+……+n</t>
+  </si>
+  <si>
+    <t>面试题47</t>
+  </si>
+  <si>
+    <t>不用加减乘除做加法</t>
+  </si>
+  <si>
+    <t>面试题48</t>
+  </si>
+  <si>
+    <t>不能被继承的类</t>
+  </si>
+  <si>
+    <t>面试题49</t>
+  </si>
+  <si>
+    <t>把字符串转换成整数</t>
+  </si>
+  <si>
+    <t>面试题50</t>
+  </si>
+  <si>
+    <t>树中两个结点的最低公共祖先</t>
+  </si>
+  <si>
+    <t>从头到尾打印链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二维数组中的查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scanf不会超时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狸猫换太子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>队列实现，不需递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串的比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用栈实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从尾到头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>递归，不能更熟悉！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已收录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈1push，栈2pop，栈2由栈1push</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>考虑0的情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通项公式迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pow(2,n)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同上上上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>善用mask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用辅助栈，top直接pop，否则push</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用辅助栈，更小值push</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左子树大于根，右子树小于根，递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用了辅助数组O(n)时间和空间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n&amp;(n-1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用栈实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意复制节点时的指针操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trick 中右左遍历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理解题意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其实考的是前序遍历和中序遍历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>递归&amp;下一个排列函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash set会TLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS,max(l,r)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左右向中间扫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意仔细。。。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约瑟夫环，f=(f+m)%i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进位为&amp; 和为^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>规律：最高位，后几位，递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>面试题34</t>
-  </si>
-  <si>
-    <t>丑数</t>
-  </si>
-  <si>
-    <t>面试题35</t>
-  </si>
-  <si>
-    <t>第一个只出现一次的字符</t>
-  </si>
-  <si>
-    <t>面试题36</t>
-  </si>
-  <si>
-    <t>数组中的逆序对</t>
-  </si>
-  <si>
-    <t>面试题37</t>
-  </si>
-  <si>
-    <t>两个链表的第一个公共结点</t>
-  </si>
-  <si>
-    <t>面试题38</t>
-  </si>
-  <si>
-    <t>数字在排序数组中出现的次数</t>
-  </si>
-  <si>
-    <t>面试题39</t>
-  </si>
-  <si>
-    <t>二叉树的深度</t>
-  </si>
-  <si>
-    <t>面试题40</t>
-  </si>
-  <si>
-    <t>数组中只出现一次的数字</t>
-  </si>
-  <si>
-    <t>面试题41</t>
-  </si>
-  <si>
-    <t>和为S的两个数字</t>
-  </si>
-  <si>
-    <t>和为S的连续正数序列</t>
-  </si>
-  <si>
-    <t>面试题42</t>
-  </si>
-  <si>
-    <t>翻转单词顺序</t>
-  </si>
-  <si>
-    <t>左旋转字符串</t>
-  </si>
-  <si>
-    <t>面试题43</t>
-  </si>
-  <si>
-    <t>N个骰子的点数</t>
-  </si>
-  <si>
-    <t>面试题44</t>
-  </si>
-  <si>
-    <t>扑克牌的顺子</t>
-  </si>
-  <si>
-    <t>面试题45</t>
-  </si>
-  <si>
-    <t>圆圈中最后剩下的数</t>
-  </si>
-  <si>
-    <t>面试题46</t>
-  </si>
-  <si>
-    <t>求1+2+……+n</t>
-  </si>
-  <si>
-    <t>面试题47</t>
-  </si>
-  <si>
-    <t>不用加减乘除做加法</t>
-  </si>
-  <si>
-    <t>面试题48</t>
-  </si>
-  <si>
-    <t>不能被继承的类</t>
-  </si>
-  <si>
-    <t>面试题49</t>
-  </si>
-  <si>
-    <t>把字符串转换成整数</t>
-  </si>
-  <si>
-    <t>面试题50</t>
-  </si>
-  <si>
-    <t>树中两个结点的最低公共祖先</t>
-  </si>
-  <si>
-    <t>从头到尾打印链表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二维数组中的查找</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scanf不会超时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狸猫换太子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>队列实现，不需递归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串的比较</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用栈实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从尾到头</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>递归，不能更熟悉！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已收录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>栈1push，栈2pop，栈2由栈1push</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>考虑0的情况</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通项公式迭代</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同上</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pow(2,n)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同上上上</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>善用mask</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用辅助栈，top直接pop，否则push</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用辅助栈，更小值push</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>左子树大于根，右子树小于根，递归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用了辅助数组O(n)时间和空间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>快慢指针</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n&amp;(n-1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用栈实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注意复制节点时的指针操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>trick 中右左遍历</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要排序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>理解题意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其实考的是前序遍历和中序遍历</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>哈希表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>递归&amp;下一个排列函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hash set会TLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS,max(l,r)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>左右向中间扫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注意仔细。。。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>约瑟夫环，f=(f+m)%i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进位为&amp; 和为^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用已有丑数找新丑数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -560,74 +564,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -640,14 +576,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -682,7 +618,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,7 +653,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -928,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A22" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -974,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -994,7 +930,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -1008,10 +944,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -1028,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
@@ -1045,7 +981,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -1075,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -1092,7 +1028,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
@@ -1109,7 +1045,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -1126,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>6</v>
@@ -1143,7 +1079,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>6</v>
@@ -1160,7 +1096,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
@@ -1177,7 +1113,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>6</v>
@@ -1194,7 +1130,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>2</v>
@@ -1211,7 +1147,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>6</v>
@@ -1228,7 +1164,7 @@
         <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>6</v>
@@ -1245,7 +1181,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>6</v>
@@ -1262,7 +1198,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>6</v>
@@ -1292,7 +1228,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>6</v>
@@ -1322,7 +1258,7 @@
         <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>6</v>
@@ -1339,7 +1275,7 @@
         <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>6</v>
@@ -1356,7 +1292,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>6</v>
@@ -1373,7 +1309,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>6</v>
@@ -1390,7 +1326,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>6</v>
@@ -1407,7 +1343,7 @@
         <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>6</v>
@@ -1424,7 +1360,7 @@
         <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>6</v>
@@ -1441,7 +1377,7 @@
         <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>6</v>
@@ -1487,14 +1423,18 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1510,21 +1450,25 @@
         <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
       <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1534,13 +1478,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>6</v>
@@ -1549,10 +1493,10 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
@@ -1562,10 +1506,10 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
@@ -1577,13 +1521,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>6</v>
@@ -1594,13 +1538,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>6</v>
@@ -1611,13 +1555,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>6</v>
@@ -1628,13 +1572,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>6</v>
@@ -1643,10 +1587,10 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
@@ -1656,10 +1600,10 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
@@ -1669,10 +1613,10 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
@@ -1682,10 +1626,10 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
@@ -1697,13 +1641,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>6</v>
@@ -1714,13 +1658,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>6</v>
@@ -1729,10 +1673,10 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
@@ -1744,13 +1688,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>6</v>
@@ -1759,10 +1703,10 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
@@ -1772,10 +1716,10 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
@@ -1785,14 +1729,14 @@
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20140513 4 new solved
</commit_message>
<xml_diff>
--- a/jzoffer.xlsx
+++ b/jzoffer.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jzoffer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5115"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
   <si>
     <t>面试题1</t>
   </si>
@@ -511,6 +506,22 @@
   </si>
   <si>
     <t>使用类的构造函数和静态变量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微软面试，nth element，也可最小堆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态维护指针和数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划，和小于零重新开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分查找，相等只能顺序</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,74 +596,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -665,14 +608,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -707,7 +650,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,7 +685,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1663,53 +1606,69 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
       <c r="B42" s="1" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E42" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1">
+        <v>1</v>
+      </c>
       <c r="B43" s="1" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="E43" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1">
+        <v>1</v>
+      </c>
       <c r="B44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1717,36 +1676,36 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
@@ -1756,10 +1715,10 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">

</xml_diff>